<commit_message>
Update README to reflect Steve's edits and minor changes to dataset
</commit_message>
<xml_diff>
--- a/data/Colorado-Watershed-Groups.xlsx
+++ b/data/Colorado-Watershed-Groups.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="13020" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Notes" sheetId="6" r:id="rId1"/>
@@ -300,7 +300,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="492">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1111" uniqueCount="493">
   <si>
     <t>Website</t>
   </si>
@@ -858,9 +858,6 @@
   </si>
   <si>
     <t>Dolores River</t>
-  </si>
-  <si>
-    <t>Republican River</t>
   </si>
   <si>
     <t>James Creek</t>
@@ -1932,6 +1929,12 @@
   </si>
   <si>
     <t xml:space="preserve">This worksheet is organized so that each document associated with a watershed group is its own record.  Therefore, the same watershed group may be listed in more than one row, but the document will be different.  </t>
+  </si>
+  <si>
+    <t>00833592</t>
+  </si>
+  <si>
+    <t>South Fork Republican River</t>
   </si>
 </sst>
 </file>
@@ -2041,7 +2044,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -2093,6 +2096,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2443,7 +2448,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
@@ -2454,12 +2459,12 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
@@ -2467,7 +2472,7 @@
     </row>
     <row r="4" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
@@ -2475,122 +2480,122 @@
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" s="16" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" s="16" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
     </row>
     <row r="9" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A9" s="16" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
     </row>
     <row r="10" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
     </row>
     <row r="11" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A11" s="16" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A12" s="16" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
     </row>
     <row r="13" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A13" s="16" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
     </row>
     <row r="14" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A14" s="16" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
     </row>
     <row r="15" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A15" s="16" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
     </row>
     <row r="16" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A16" s="16" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A17" s="16" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A18" s="16" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A25" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A27" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.25">
@@ -2598,22 +2603,22 @@
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
     </row>
     <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
     </row>
     <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
     </row>
     <row r="35" spans="1:1" x14ac:dyDescent="0.25">
@@ -2621,7 +2626,7 @@
     </row>
     <row r="36" spans="1:1" ht="135" x14ac:dyDescent="0.25">
       <c r="A36" s="4" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
     <row r="37" spans="1:1" x14ac:dyDescent="0.25">
@@ -2629,7 +2634,7 @@
     </row>
     <row r="38" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A38" s="4" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.25">
@@ -2637,7 +2642,7 @@
     </row>
     <row r="40" spans="1:1" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="4" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="41" spans="1:1" x14ac:dyDescent="0.25">
@@ -2645,22 +2650,22 @@
     </row>
     <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="6" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
     </row>
     <row r="44" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
     </row>
     <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" spans="1:1" x14ac:dyDescent="0.25">
@@ -2668,22 +2673,22 @@
     </row>
     <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="6" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
     </row>
     <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
     </row>
     <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="51" spans="1:1" x14ac:dyDescent="0.25">
@@ -2691,22 +2696,22 @@
     </row>
     <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="6" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="30" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
     </row>
     <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
     </row>
     <row r="56" spans="1:1" x14ac:dyDescent="0.25">
@@ -2714,12 +2719,12 @@
     </row>
     <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
     </row>
     <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
     </row>
     <row r="59" spans="1:1" x14ac:dyDescent="0.25">
@@ -2727,12 +2732,12 @@
     </row>
     <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
     </row>
     <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
     </row>
   </sheetData>
@@ -2745,22 +2750,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M86"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H56" sqref="H56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="54" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="53.7109375" customWidth="1"/>
-    <col min="4" max="4" width="18.42578125" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" customWidth="1"/>
+    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="36.85546875" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.140625" customWidth="1"/>
     <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" customWidth="1"/>
-    <col min="9" max="10" width="31.85546875" customWidth="1"/>
+    <col min="8" max="8" width="15" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="42.85546875" customWidth="1"/>
     <col min="12" max="12" width="15.28515625" customWidth="1"/>
     <col min="13" max="13" width="47.42578125" bestFit="1" customWidth="1"/>
@@ -2771,40 +2777,40 @@
         <v>130</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>290</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>474</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>291</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>475</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>292</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>476</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>293</v>
-      </c>
       <c r="H1" s="1" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>148</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="K1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2812,34 +2818,34 @@
         <v>19</v>
       </c>
       <c r="B2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C2" t="s">
         <v>181</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F2" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G2">
         <v>13010002</v>
       </c>
       <c r="H2" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I2" t="s">
         <v>159</v>
       </c>
       <c r="J2" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L2" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
@@ -2847,32 +2853,32 @@
         <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C3" t="s">
         <v>181</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F3" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I3" t="s">
         <v>159</v>
       </c>
       <c r="J3" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L3" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -2880,31 +2886,31 @@
         <v>21</v>
       </c>
       <c r="B4" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="C4" t="s">
         <v>182</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F4" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G4">
         <v>14080104</v>
       </c>
       <c r="H4" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I4" t="s">
         <v>169</v>
       </c>
       <c r="J4" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>22</v>
@@ -2916,31 +2922,31 @@
         <v>23</v>
       </c>
       <c r="B5" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C5" t="s">
         <v>182</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="F5" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G5">
         <v>14080104</v>
       </c>
       <c r="H5" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I5" t="s">
         <v>169</v>
       </c>
       <c r="J5" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>24</v>
@@ -2952,29 +2958,29 @@
         <v>25</v>
       </c>
       <c r="B6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="C6" t="s">
         <v>183</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F6" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I6" t="s">
         <v>132</v>
       </c>
       <c r="J6" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>26</v>
@@ -2983,34 +2989,34 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="C7" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F7" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G7">
         <v>10190003</v>
       </c>
       <c r="H7" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I7" t="s">
         <v>152</v>
       </c>
       <c r="J7" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>27</v>
@@ -3022,31 +3028,31 @@
         <v>28</v>
       </c>
       <c r="B8" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="C8" t="s">
         <v>184</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F8" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G8">
         <v>10190002</v>
       </c>
       <c r="H8" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I8" t="s">
         <v>152</v>
       </c>
       <c r="J8" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>29</v>
@@ -3058,31 +3064,31 @@
         <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="C9" t="s">
         <v>172</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="F9" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G9">
         <v>10190003</v>
       </c>
       <c r="H9" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="I9" t="s">
         <v>481</v>
       </c>
-      <c r="I9" t="s">
-        <v>482</v>
-      </c>
       <c r="J9" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>31</v>
@@ -3094,31 +3100,31 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="C10" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F10" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G10">
         <v>10190006</v>
       </c>
       <c r="H10" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I10" t="s">
         <v>162</v>
       </c>
       <c r="J10" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>2</v>
@@ -3130,31 +3136,31 @@
         <v>32</v>
       </c>
       <c r="B11" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="C11" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D11" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="F11" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G11">
         <v>10190006</v>
       </c>
       <c r="H11" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I11" t="s">
         <v>162</v>
       </c>
       <c r="J11" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>33</v>
@@ -3166,31 +3172,31 @@
         <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="C12" t="s">
         <v>173</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F12" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G12">
         <v>14010002</v>
       </c>
       <c r="H12" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I12" t="s">
         <v>136</v>
       </c>
       <c r="J12" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>35</v>
@@ -3202,31 +3208,31 @@
         <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C13" t="s">
         <v>174</v>
       </c>
       <c r="D13" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="F13" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G13">
         <v>10190005</v>
       </c>
       <c r="H13" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I13" t="s">
         <v>162</v>
       </c>
       <c r="J13" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K13" s="2" t="s">
         <v>37</v>
@@ -3238,31 +3244,31 @@
         <v>38</v>
       </c>
       <c r="B14" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="C14" t="s">
+        <v>296</v>
+      </c>
+      <c r="D14" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="E14" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="D14" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E14" s="3" t="s">
-        <v>298</v>
-      </c>
       <c r="F14" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G14">
         <v>10190003</v>
       </c>
       <c r="H14" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I14" t="s">
         <v>152</v>
       </c>
       <c r="J14" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K14" s="2" t="s">
         <v>39</v>
@@ -3274,31 +3280,31 @@
         <v>40</v>
       </c>
       <c r="B15" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="C15" t="s">
         <v>175</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="F15" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G15">
         <v>10190003</v>
       </c>
       <c r="H15" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I15" t="s">
         <v>152</v>
       </c>
       <c r="J15" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K15" s="2" t="s">
         <v>41</v>
@@ -3310,31 +3316,31 @@
         <v>42</v>
       </c>
       <c r="B16" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="C16" t="s">
         <v>176</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F16" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G16">
         <v>10190004</v>
       </c>
       <c r="H16" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I16" t="s">
         <v>162</v>
       </c>
       <c r="J16" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K16" s="2" t="s">
         <v>43</v>
@@ -3346,31 +3352,31 @@
         <v>3</v>
       </c>
       <c r="B17" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C17" t="s">
         <v>177</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="F17" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G17">
         <v>10190005</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I17" t="s">
         <v>162</v>
       </c>
       <c r="J17" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K17" s="2" t="s">
         <v>4</v>
@@ -3382,31 +3388,31 @@
         <v>44</v>
       </c>
       <c r="B18" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="C18" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="F18" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G18">
         <v>14020001</v>
       </c>
       <c r="H18" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I18" t="s">
         <v>144</v>
       </c>
       <c r="J18" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K18" s="2" t="s">
         <v>45</v>
@@ -3418,31 +3424,31 @@
         <v>5</v>
       </c>
       <c r="B19" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="C19" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D19" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F19" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G19">
         <v>10190007</v>
       </c>
       <c r="H19" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I19" t="s">
         <v>162</v>
       </c>
       <c r="J19" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K19" s="2" t="s">
         <v>6</v>
@@ -3454,31 +3460,31 @@
         <v>46</v>
       </c>
       <c r="B20" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C20" t="s">
+        <v>288</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="D20" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>290</v>
-      </c>
       <c r="F20" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="H20" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I20" t="s">
         <v>162</v>
       </c>
       <c r="J20" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>47</v>
@@ -3490,28 +3496,28 @@
         <v>48</v>
       </c>
       <c r="B21" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="C21" s="20"/>
       <c r="D21" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E21" s="22"/>
       <c r="F21" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I21" t="s">
         <v>132</v>
       </c>
       <c r="J21" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L21" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.25">
@@ -3519,31 +3525,31 @@
         <v>49</v>
       </c>
       <c r="B22" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="C22" t="s">
         <v>185</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F22" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G22">
         <v>14030004</v>
       </c>
       <c r="H22" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I22" t="s">
         <v>169</v>
       </c>
       <c r="J22" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>50</v>
@@ -3555,32 +3561,32 @@
         <v>51</v>
       </c>
       <c r="B23" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="C23" t="s">
         <v>185</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F23" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I23" t="s">
         <v>169</v>
       </c>
       <c r="J23" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L23" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
@@ -3588,29 +3594,29 @@
         <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="C24" t="s">
         <v>178</v>
       </c>
       <c r="D24" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E24" s="22"/>
       <c r="F24" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G24">
         <v>14010003</v>
       </c>
       <c r="H24" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I24" t="s">
         <v>136</v>
       </c>
       <c r="J24" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K24" s="2" t="s">
         <v>53</v>
@@ -3622,31 +3628,31 @@
         <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="C25" t="s">
         <v>185</v>
       </c>
       <c r="D25" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="F25" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G25">
         <v>14030002</v>
       </c>
       <c r="H25" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I25" t="s">
         <v>169</v>
       </c>
       <c r="J25" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>55</v>
@@ -3658,31 +3664,31 @@
         <v>7</v>
       </c>
       <c r="B26" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="C26" t="s">
+        <v>300</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>301</v>
       </c>
-      <c r="D26" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>302</v>
-      </c>
       <c r="F26" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G26">
         <v>10190006</v>
       </c>
       <c r="H26" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I26" t="s">
         <v>162</v>
       </c>
       <c r="J26" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K26" s="2" t="s">
         <v>8</v>
@@ -3694,29 +3700,29 @@
         <v>56</v>
       </c>
       <c r="B27" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="C27" t="s">
         <v>179</v>
       </c>
       <c r="D27" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F27" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G27" s="20"/>
       <c r="H27" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I27" t="s">
         <v>132</v>
       </c>
       <c r="J27" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K27" s="2" t="s">
         <v>57</v>
@@ -3728,31 +3734,31 @@
         <v>135</v>
       </c>
       <c r="B28" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="C28" t="s">
         <v>179</v>
       </c>
       <c r="D28" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="F28" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G28">
         <v>11020003</v>
       </c>
       <c r="H28" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I28" t="s">
         <v>132</v>
       </c>
       <c r="J28" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K28" s="2" t="s">
         <v>58</v>
@@ -3764,31 +3770,31 @@
         <v>9</v>
       </c>
       <c r="B29" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="C29" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="D29" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="F29" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G29">
         <v>10190005</v>
       </c>
       <c r="H29" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I29" t="s">
         <v>162</v>
       </c>
       <c r="J29" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K29" s="2" t="s">
         <v>10</v>
@@ -3800,29 +3806,29 @@
         <v>59</v>
       </c>
       <c r="B30" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="C30" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D30" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="F30" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G30" s="20"/>
       <c r="H30" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I30" t="s">
         <v>136</v>
       </c>
       <c r="J30" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K30" s="2" t="s">
         <v>60</v>
@@ -3834,29 +3840,29 @@
         <v>61</v>
       </c>
       <c r="B31" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="C31" t="s">
         <v>173</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E31" s="3" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="F31" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I31" t="s">
         <v>136</v>
       </c>
       <c r="J31" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K31" s="2" t="s">
         <v>62</v>
@@ -3868,31 +3874,31 @@
         <v>63</v>
       </c>
       <c r="B32" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="C32" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D32" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F32" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G32">
         <v>10190007</v>
       </c>
       <c r="H32" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I32" t="s">
         <v>162</v>
       </c>
       <c r="J32" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>166</v>
@@ -3904,30 +3910,30 @@
         <v>64</v>
       </c>
       <c r="B33" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="C33" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D33" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E33" s="22"/>
       <c r="F33" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I33" t="s">
         <v>144</v>
       </c>
       <c r="J33" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L33" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.25">
@@ -3935,27 +3941,27 @@
         <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="C34" t="s">
         <v>134</v>
       </c>
       <c r="D34" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E34" s="22"/>
       <c r="F34" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I34" t="s">
         <v>131</v>
       </c>
       <c r="J34" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>66</v>
@@ -3967,25 +3973,25 @@
         <v>138</v>
       </c>
       <c r="B35" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="C35" s="20"/>
       <c r="D35" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E35" s="22"/>
       <c r="F35" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I35" t="s">
         <v>136</v>
       </c>
       <c r="J35" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>139</v>
@@ -3997,27 +4003,27 @@
         <v>140</v>
       </c>
       <c r="B36" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="C36" t="s">
         <v>180</v>
       </c>
       <c r="D36" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E36" s="22"/>
       <c r="F36" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G36" s="20"/>
       <c r="H36" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I36" t="s">
         <v>136</v>
       </c>
       <c r="J36" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K36" s="2" t="s">
         <v>141</v>
@@ -4029,22 +4035,22 @@
         <v>67</v>
       </c>
       <c r="B37" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C37" s="20"/>
       <c r="E37" s="22"/>
       <c r="F37" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G37" s="20"/>
       <c r="H37" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I37" t="s">
         <v>136</v>
       </c>
       <c r="J37" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K37" s="2" t="s">
         <v>68</v>
@@ -4056,29 +4062,29 @@
         <v>69</v>
       </c>
       <c r="B38" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C38" t="s">
         <v>183</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F38" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G38" s="20"/>
       <c r="H38" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I38" t="s">
         <v>132</v>
       </c>
       <c r="J38" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K38" s="2" t="s">
         <v>70</v>
@@ -4090,31 +4096,31 @@
         <v>153</v>
       </c>
       <c r="B39" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="C39" t="s">
         <v>184</v>
       </c>
       <c r="D39" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E39" s="3" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="F39" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G39">
         <v>10190002</v>
       </c>
       <c r="H39" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I39" t="s">
         <v>152</v>
       </c>
       <c r="J39" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>154</v>
@@ -4126,29 +4132,29 @@
         <v>145</v>
       </c>
       <c r="B40" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="C40" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="D40" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E40" s="22"/>
       <c r="F40" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G40">
         <v>14020005</v>
       </c>
       <c r="H40" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I40" t="s">
         <v>144</v>
       </c>
       <c r="J40" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K40" s="2" t="s">
         <v>146</v>
@@ -4160,32 +4166,32 @@
         <v>71</v>
       </c>
       <c r="B41" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C41" s="20"/>
       <c r="D41" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E41" s="22"/>
       <c r="F41" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I41" t="s">
         <v>144</v>
       </c>
       <c r="J41" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K41" s="2" t="s">
         <v>72</v>
       </c>
       <c r="L41" s="19"/>
       <c r="M41" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.25">
@@ -4193,31 +4199,31 @@
         <v>73</v>
       </c>
       <c r="B42" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C42" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="F42" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G42">
         <v>10190005</v>
       </c>
       <c r="H42" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I42" t="s">
         <v>162</v>
       </c>
       <c r="J42" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>74</v>
@@ -4229,31 +4235,31 @@
         <v>167</v>
       </c>
       <c r="B43" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="C43" t="s">
+        <v>304</v>
+      </c>
+      <c r="D43" s="18" t="s">
+        <v>480</v>
+      </c>
+      <c r="E43" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="D43" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E43" s="3" t="s">
-        <v>306</v>
-      </c>
       <c r="F43" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G43">
         <v>10190005</v>
       </c>
       <c r="H43" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I43" t="s">
         <v>162</v>
       </c>
       <c r="J43" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K43" s="2" t="s">
         <v>168</v>
@@ -4265,31 +4271,31 @@
         <v>160</v>
       </c>
       <c r="B44" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="C44" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="D44" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="F44" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G44">
         <v>13010003</v>
       </c>
       <c r="H44" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I44" t="s">
         <v>159</v>
       </c>
       <c r="J44" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K44" s="2" t="s">
         <v>161</v>
@@ -4301,29 +4307,29 @@
         <v>75</v>
       </c>
       <c r="B45" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="C45" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="D45" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E45" s="22"/>
       <c r="F45" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G45">
         <v>14020005</v>
       </c>
       <c r="H45" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I45" t="s">
         <v>144</v>
       </c>
       <c r="J45" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>76</v>
@@ -4335,29 +4341,29 @@
         <v>77</v>
       </c>
       <c r="B46" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="C46" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="D46" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E46" s="22"/>
       <c r="F46" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G46">
         <v>11020002</v>
       </c>
       <c r="H46" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I46" t="s">
         <v>147</v>
       </c>
       <c r="J46" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>78</v>
@@ -4369,25 +4375,25 @@
         <v>79</v>
       </c>
       <c r="B47" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="C47" s="20"/>
       <c r="D47" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E47" s="22"/>
       <c r="F47" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G47" s="20"/>
       <c r="H47" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I47" t="s">
         <v>132</v>
       </c>
       <c r="J47" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>80</v>
@@ -4399,31 +4405,31 @@
         <v>11</v>
       </c>
       <c r="B48" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="C48" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="D48" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="F48" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G48">
         <v>10190005</v>
       </c>
       <c r="H48" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I48" t="s">
         <v>162</v>
       </c>
       <c r="J48" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>12</v>
@@ -4435,31 +4441,31 @@
         <v>13</v>
       </c>
       <c r="B49" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C49" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D49" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="F49" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G49">
         <v>10190005</v>
       </c>
       <c r="H49" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I49" t="s">
         <v>162</v>
       </c>
       <c r="J49" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K49" s="2" t="s">
         <v>14</v>
@@ -4471,31 +4477,31 @@
         <v>81</v>
       </c>
       <c r="B50" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="C50" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D50" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F50" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G50">
         <v>14010006</v>
       </c>
       <c r="H50" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I50" t="s">
         <v>136</v>
       </c>
       <c r="J50" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>82</v>
@@ -4507,31 +4513,31 @@
         <v>15</v>
       </c>
       <c r="B51" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="C51" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F51" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G51">
         <v>10190003</v>
       </c>
       <c r="H51" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I51" t="s">
         <v>162</v>
       </c>
       <c r="J51" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K51" s="2" t="s">
         <v>16</v>
@@ -4543,25 +4549,25 @@
         <v>142</v>
       </c>
       <c r="B52" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="C52" s="20"/>
       <c r="D52" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E52" s="22"/>
       <c r="F52" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G52" s="20"/>
       <c r="H52" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I52" t="s">
         <v>136</v>
       </c>
       <c r="J52" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K52" s="2" t="s">
         <v>143</v>
@@ -4573,29 +4579,29 @@
         <v>83</v>
       </c>
       <c r="B53" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="C53" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D53" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E53" s="22"/>
       <c r="F53" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G53" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="H53" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I53" t="s">
         <v>133</v>
       </c>
       <c r="J53" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K53" s="2" t="s">
         <v>84</v>
@@ -4607,29 +4613,29 @@
         <v>85</v>
       </c>
       <c r="B54" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="C54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D54" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G54">
         <v>14080101</v>
       </c>
       <c r="H54" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I54" t="s">
         <v>169</v>
       </c>
       <c r="J54" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K54" s="2" t="s">
         <v>170</v>
@@ -4641,31 +4647,31 @@
         <v>86</v>
       </c>
       <c r="B55" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="C55" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F55" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G55">
         <v>11020010</v>
       </c>
       <c r="H55" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I55" t="s">
         <v>132</v>
       </c>
       <c r="J55" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K55" s="2" t="s">
         <v>87</v>
@@ -4677,31 +4683,35 @@
         <v>88</v>
       </c>
       <c r="B56" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="C56" t="s">
-        <v>186</v>
+        <v>492</v>
       </c>
       <c r="D56" s="18" t="s">
-        <v>481</v>
-      </c>
-      <c r="E56" s="22"/>
+        <v>480</v>
+      </c>
+      <c r="E56" s="23" t="s">
+        <v>491</v>
+      </c>
       <c r="F56" s="21" t="s">
-        <v>483</v>
-      </c>
-      <c r="G56" s="20"/>
+        <v>480</v>
+      </c>
+      <c r="G56" s="24">
+        <v>10250003</v>
+      </c>
       <c r="H56" s="18" t="s">
-        <v>483</v>
+        <v>480</v>
       </c>
       <c r="I56" t="s">
         <v>132</v>
       </c>
       <c r="J56" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K56" s="2"/>
       <c r="L56" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="57" spans="1:12" x14ac:dyDescent="0.25">
@@ -4709,25 +4719,25 @@
         <v>150</v>
       </c>
       <c r="B57" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="C57" s="20"/>
       <c r="D57" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E57" s="22"/>
       <c r="F57" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G57" s="20"/>
       <c r="H57" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I57" t="s">
         <v>144</v>
       </c>
       <c r="J57" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K57" s="2" t="s">
         <v>149</v>
@@ -4739,29 +4749,29 @@
         <v>164</v>
       </c>
       <c r="B58" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="C58" t="s">
         <v>159</v>
       </c>
       <c r="D58" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F58" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G58" s="20"/>
       <c r="H58" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I58" t="s">
         <v>159</v>
       </c>
       <c r="J58" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K58" s="2" t="s">
         <v>165</v>
@@ -4773,31 +4783,31 @@
         <v>89</v>
       </c>
       <c r="B59" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="C59" t="s">
         <v>159</v>
       </c>
       <c r="D59" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F59" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G59">
         <v>13010000</v>
       </c>
       <c r="H59" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I59" t="s">
         <v>159</v>
       </c>
       <c r="J59" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>90</v>
@@ -4809,25 +4819,25 @@
         <v>91</v>
       </c>
       <c r="B60" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="C60" s="20"/>
       <c r="D60" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E60" s="22"/>
       <c r="F60" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G60" s="20"/>
       <c r="H60" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I60" t="s">
         <v>169</v>
       </c>
       <c r="J60" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K60" s="2" t="s">
         <v>92</v>
@@ -4839,31 +4849,31 @@
         <v>93</v>
       </c>
       <c r="B61" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="C61" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F61" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G61">
         <v>14010004</v>
       </c>
       <c r="H61" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I61" t="s">
         <v>136</v>
       </c>
       <c r="J61" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K61" s="2" t="s">
         <v>94</v>
@@ -4875,25 +4885,25 @@
         <v>95</v>
       </c>
       <c r="B62" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="C62" s="20"/>
       <c r="D62" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E62" s="22"/>
       <c r="F62" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G62" s="20"/>
       <c r="H62" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I62" t="s">
         <v>132</v>
       </c>
       <c r="J62" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K62" s="2" t="s">
         <v>96</v>
@@ -4905,25 +4915,25 @@
         <v>97</v>
       </c>
       <c r="B63" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="C63" s="20"/>
       <c r="D63" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E63" s="22"/>
       <c r="F63" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G63" s="20"/>
       <c r="H63" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I63" t="s">
         <v>169</v>
       </c>
       <c r="J63" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K63" s="2" t="s">
         <v>98</v>
@@ -4935,25 +4945,25 @@
         <v>171</v>
       </c>
       <c r="B64" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="C64" s="20"/>
       <c r="D64" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E64" s="22"/>
       <c r="F64" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G64" s="20"/>
       <c r="H64" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I64" t="s">
         <v>169</v>
       </c>
       <c r="J64" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K64" s="2" t="s">
         <v>170</v>
@@ -4965,25 +4975,25 @@
         <v>99</v>
       </c>
       <c r="B65" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="C65" s="20"/>
       <c r="D65" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E65" s="22"/>
       <c r="F65" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G65" s="20"/>
       <c r="H65" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I65" t="s">
         <v>159</v>
       </c>
       <c r="J65" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K65" s="2" t="s">
         <v>100</v>
@@ -4995,28 +5005,28 @@
         <v>101</v>
       </c>
       <c r="B66" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="C66" s="20"/>
       <c r="D66" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E66" s="22"/>
       <c r="F66" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G66" s="20"/>
       <c r="H66" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I66" t="s">
         <v>159</v>
       </c>
       <c r="J66" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L66" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.25">
@@ -5024,31 +5034,31 @@
         <v>102</v>
       </c>
       <c r="B67" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C67" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F67" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G67">
         <v>14030003</v>
       </c>
       <c r="H67" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I67" t="s">
         <v>169</v>
       </c>
       <c r="J67" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K67" s="2" t="s">
         <v>103</v>
@@ -5060,31 +5070,31 @@
         <v>155</v>
       </c>
       <c r="B68" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="C68" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D68" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="F68" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G68">
         <v>10190003</v>
       </c>
       <c r="H68" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I68" t="s">
         <v>152</v>
       </c>
       <c r="J68" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K68" s="2" t="s">
         <v>156</v>
@@ -5096,31 +5106,31 @@
         <v>104</v>
       </c>
       <c r="B69" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="C69" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="D69" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E69" s="3" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="F69" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G69">
         <v>10190007</v>
       </c>
       <c r="H69" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I69" t="s">
         <v>162</v>
       </c>
       <c r="J69" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K69" s="2" t="s">
         <v>105</v>
@@ -5132,31 +5142,31 @@
         <v>106</v>
       </c>
       <c r="B70" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="C70" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="D70" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E70" s="3" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G70">
         <v>14010002</v>
       </c>
       <c r="H70" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I70" t="s">
         <v>136</v>
       </c>
       <c r="J70" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K70" s="2" t="s">
         <v>107</v>
@@ -5168,31 +5178,31 @@
         <v>108</v>
       </c>
       <c r="B71" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="C71" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D71" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E71" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G71" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="H71" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I71" t="s">
         <v>162</v>
       </c>
       <c r="J71" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K71" s="2" t="s">
         <v>109</v>
@@ -5204,31 +5214,31 @@
         <v>17</v>
       </c>
       <c r="B72" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="C72" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D72" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G72">
         <v>10190005</v>
       </c>
       <c r="H72" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I72" t="s">
         <v>162</v>
       </c>
       <c r="J72" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K72" s="2" t="s">
         <v>18</v>
@@ -5240,31 +5250,31 @@
         <v>110</v>
       </c>
       <c r="B73" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="C73" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="D73" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G73">
         <v>10190005</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I73" t="s">
         <v>162</v>
       </c>
       <c r="J73" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K73" s="2" t="s">
         <v>111</v>
@@ -5276,25 +5286,25 @@
         <v>112</v>
       </c>
       <c r="B74" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="C74" s="20"/>
       <c r="D74" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E74" s="22"/>
       <c r="F74" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G74" s="20"/>
       <c r="H74" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I74" t="s">
         <v>136</v>
       </c>
       <c r="J74" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K74" s="2" t="s">
         <v>113</v>
@@ -5306,31 +5316,31 @@
         <v>114</v>
       </c>
       <c r="B75" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="C75" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="D75" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G75" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I75" t="s">
         <v>152</v>
       </c>
       <c r="J75" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K75" s="2" t="s">
         <v>157</v>
@@ -5342,29 +5352,29 @@
         <v>117</v>
       </c>
       <c r="B76" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="C76" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D76" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G76" s="20"/>
       <c r="H76" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I76" t="s">
         <v>136</v>
       </c>
       <c r="J76" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K76" s="2" t="s">
         <v>118</v>
@@ -5376,25 +5386,25 @@
         <v>151</v>
       </c>
       <c r="B77" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="C77" s="20"/>
       <c r="D77" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E77" s="22"/>
       <c r="F77" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G77" s="20"/>
       <c r="H77" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I77" t="s">
         <v>144</v>
       </c>
       <c r="J77" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K77" s="2" t="s">
         <v>120</v>
@@ -5406,35 +5416,35 @@
         <v>119</v>
       </c>
       <c r="B78" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C78" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D78" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G78">
         <v>14020006</v>
       </c>
       <c r="H78" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I78" t="s">
         <v>144</v>
       </c>
       <c r="J78" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K78" s="2"/>
       <c r="L78" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.25">
@@ -5442,32 +5452,32 @@
         <v>137</v>
       </c>
       <c r="B79" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C79" t="s">
         <v>183</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E79" s="3" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G79" s="20"/>
       <c r="H79" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I79" t="s">
         <v>132</v>
       </c>
       <c r="J79" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L79" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.25">
@@ -5475,34 +5485,34 @@
         <v>121</v>
       </c>
       <c r="B80" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="C80" t="s">
         <v>176</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G80">
         <v>10190004</v>
       </c>
       <c r="H80" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I80" t="s">
         <v>162</v>
       </c>
       <c r="J80" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L80" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.25">
@@ -5510,31 +5520,31 @@
         <v>122</v>
       </c>
       <c r="B81" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="C81" t="s">
         <v>134</v>
       </c>
       <c r="D81" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G81">
         <v>14050001</v>
       </c>
       <c r="H81" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I81" t="s">
         <v>131</v>
       </c>
       <c r="J81" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K81" s="2" t="s">
         <v>123</v>
@@ -5546,27 +5556,27 @@
         <v>124</v>
       </c>
       <c r="B82" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="C82" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D82" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E82" s="22"/>
       <c r="F82" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G82" s="20"/>
       <c r="H82" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I82" t="s">
         <v>169</v>
       </c>
       <c r="J82" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K82" s="2" t="s">
         <v>125</v>
@@ -5578,25 +5588,25 @@
         <v>126</v>
       </c>
       <c r="B83" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="C83" s="20"/>
       <c r="D83" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="E83" s="22"/>
       <c r="F83" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G83" s="20"/>
       <c r="H83" s="18" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="I83" t="s">
         <v>136</v>
       </c>
       <c r="J83" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K83" s="2" t="s">
         <v>127</v>
@@ -5608,34 +5618,34 @@
         <v>158</v>
       </c>
       <c r="B84" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="C84" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="D84" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="G84">
         <v>10190003</v>
       </c>
       <c r="H84" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I84" t="s">
         <v>152</v>
       </c>
       <c r="J84" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="L84" s="18" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="85" spans="1:12" x14ac:dyDescent="0.25">
@@ -5643,29 +5653,29 @@
         <v>115</v>
       </c>
       <c r="B85" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="C85" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D85" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E85" s="22"/>
       <c r="F85" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G85">
         <v>14020004</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I85" t="s">
         <v>144</v>
       </c>
       <c r="J85" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K85" s="2" t="s">
         <v>116</v>
@@ -5677,29 +5687,29 @@
         <v>128</v>
       </c>
       <c r="B86" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="C86" t="s">
         <v>163</v>
       </c>
       <c r="D86" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="E86" s="22"/>
       <c r="F86" s="21" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="G86">
         <v>13010003</v>
       </c>
       <c r="H86" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="I86" t="s">
         <v>159</v>
       </c>
       <c r="J86" s="18" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="K86" s="2" t="s">
         <v>129</v>
@@ -6043,16 +6053,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>130</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>0</v>
@@ -6067,13 +6077,13 @@
         <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D2">
         <v>2005</v>
       </c>
       <c r="E2" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -6085,13 +6095,13 @@
         <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D3">
         <v>2013</v>
       </c>
       <c r="E3" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -6103,13 +6113,13 @@
         <v>23</v>
       </c>
       <c r="C4" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D4">
         <v>2011</v>
       </c>
       <c r="E4" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -6118,16 +6128,16 @@
         <v>BarrLakeMiltonReservoirWA</v>
       </c>
       <c r="B5" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C5" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D5">
         <v>2008</v>
       </c>
       <c r="E5" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -6139,13 +6149,13 @@
         <v>28</v>
       </c>
       <c r="C6" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D6">
         <v>2014</v>
       </c>
       <c r="E6" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -6157,13 +6167,13 @@
         <v>30</v>
       </c>
       <c r="C7" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D7">
         <v>2002</v>
       </c>
       <c r="E7" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -6175,13 +6185,13 @@
         <v>32</v>
       </c>
       <c r="C8" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D8">
         <v>2007</v>
       </c>
       <c r="E8" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -6193,13 +6203,13 @@
         <v>32</v>
       </c>
       <c r="C9" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D9">
         <v>2010</v>
       </c>
       <c r="E9" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -6211,13 +6221,13 @@
         <v>34</v>
       </c>
       <c r="C10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D10">
         <v>2013</v>
       </c>
       <c r="E10" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -6229,13 +6239,13 @@
         <v>36</v>
       </c>
       <c r="C11" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D11">
         <v>2007</v>
       </c>
       <c r="E11" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -6247,13 +6257,13 @@
         <v>38</v>
       </c>
       <c r="C12" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D12">
         <v>2014</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -6265,13 +6275,13 @@
         <v>42</v>
       </c>
       <c r="C13" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D13">
         <v>2007</v>
       </c>
       <c r="E13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -6283,13 +6293,13 @@
         <v>3</v>
       </c>
       <c r="C14" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D14">
         <v>2014</v>
       </c>
       <c r="E14" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -6301,13 +6311,13 @@
         <v>44</v>
       </c>
       <c r="C15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D15">
         <v>2005</v>
       </c>
       <c r="E15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -6319,13 +6329,13 @@
         <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D16">
         <v>2014</v>
       </c>
       <c r="E16" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -6337,10 +6347,10 @@
         <v>5</v>
       </c>
       <c r="C17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -6352,13 +6362,13 @@
         <v>46</v>
       </c>
       <c r="C18" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D18">
         <v>2011</v>
       </c>
       <c r="E18" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -6370,13 +6380,13 @@
         <v>46</v>
       </c>
       <c r="C19" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D19">
         <v>2011</v>
       </c>
       <c r="E19" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -6388,13 +6398,13 @@
         <v>46</v>
       </c>
       <c r="C20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D20">
         <v>2013</v>
       </c>
       <c r="E20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -6406,13 +6416,13 @@
         <v>46</v>
       </c>
       <c r="C21" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D21">
         <v>2014</v>
       </c>
       <c r="E21" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -6424,13 +6434,13 @@
         <v>49</v>
       </c>
       <c r="C22" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D22">
         <v>2013</v>
       </c>
       <c r="E22" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -6442,13 +6452,13 @@
         <v>52</v>
       </c>
       <c r="C23" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D23">
         <v>2013</v>
       </c>
       <c r="E23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -6460,13 +6470,13 @@
         <v>52</v>
       </c>
       <c r="C24" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D24">
         <v>1996</v>
       </c>
       <c r="E24" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -6478,13 +6488,13 @@
         <v>52</v>
       </c>
       <c r="C25" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D25">
         <v>2013</v>
       </c>
       <c r="E25" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -6496,13 +6506,13 @@
         <v>54</v>
       </c>
       <c r="C26" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D26">
         <v>2006</v>
       </c>
       <c r="E26" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -6514,13 +6524,13 @@
         <v>7</v>
       </c>
       <c r="C27" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D27">
         <v>2014</v>
       </c>
       <c r="E27" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -6532,13 +6542,13 @@
         <v>7</v>
       </c>
       <c r="C28" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D28">
         <v>2014</v>
       </c>
       <c r="E28" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -6550,13 +6560,13 @@
         <v>135</v>
       </c>
       <c r="C29" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D29">
         <v>2011</v>
       </c>
       <c r="E29" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -6568,10 +6578,10 @@
         <v>153</v>
       </c>
       <c r="C30" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E30" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -6583,13 +6593,13 @@
         <v>145</v>
       </c>
       <c r="C31" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D31">
         <v>2009</v>
       </c>
       <c r="E31" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -6601,10 +6611,10 @@
         <v>167</v>
       </c>
       <c r="C32" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E32" s="2" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -6616,13 +6626,13 @@
         <v>160</v>
       </c>
       <c r="C33" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D33">
         <v>2010</v>
       </c>
       <c r="E33" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -6634,13 +6644,13 @@
         <v>75</v>
       </c>
       <c r="C34" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D34">
         <v>2012</v>
       </c>
       <c r="E34" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -6652,13 +6662,13 @@
         <v>75</v>
       </c>
       <c r="C35" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D35">
         <v>2012</v>
       </c>
       <c r="E35" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -6670,13 +6680,13 @@
         <v>77</v>
       </c>
       <c r="C36" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D36">
         <v>2012</v>
       </c>
       <c r="E36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -6688,13 +6698,13 @@
         <v>11</v>
       </c>
       <c r="C37" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D37">
         <v>2014</v>
       </c>
       <c r="E37" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -6706,13 +6716,13 @@
         <v>11</v>
       </c>
       <c r="C38" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D38">
         <v>2005</v>
       </c>
       <c r="E38" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -6724,13 +6734,13 @@
         <v>13</v>
       </c>
       <c r="C39" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D39">
         <v>2014</v>
       </c>
       <c r="E39" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -6742,10 +6752,10 @@
         <v>81</v>
       </c>
       <c r="C40" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="E40" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -6757,13 +6767,13 @@
         <v>83</v>
       </c>
       <c r="C41" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D41">
         <v>2012</v>
       </c>
       <c r="E41" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -6775,13 +6785,13 @@
         <v>83</v>
       </c>
       <c r="C42" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D42">
         <v>2012</v>
       </c>
       <c r="E42" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -6793,13 +6803,13 @@
         <v>85</v>
       </c>
       <c r="C43" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D43">
         <v>2008</v>
       </c>
       <c r="E43" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -6811,13 +6821,13 @@
         <v>86</v>
       </c>
       <c r="C44" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D44">
         <v>2014</v>
       </c>
       <c r="E44" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -6829,13 +6839,13 @@
         <v>89</v>
       </c>
       <c r="C45" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D45">
         <v>2007</v>
       </c>
       <c r="E45" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -6847,13 +6857,13 @@
         <v>89</v>
       </c>
       <c r="C46" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D46">
         <v>2014</v>
       </c>
       <c r="E46" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -6865,13 +6875,13 @@
         <v>93</v>
       </c>
       <c r="C47" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D47">
         <v>2008</v>
       </c>
       <c r="E47" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -6883,13 +6893,13 @@
         <v>93</v>
       </c>
       <c r="C48" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D48">
         <v>2012</v>
       </c>
       <c r="E48" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -6901,13 +6911,13 @@
         <v>102</v>
       </c>
       <c r="C49" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D49">
         <v>1998</v>
       </c>
       <c r="E49" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -6919,13 +6929,13 @@
         <v>106</v>
       </c>
       <c r="C50" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D50">
         <v>2013</v>
       </c>
       <c r="E50" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -6937,13 +6947,13 @@
         <v>119</v>
       </c>
       <c r="C51" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D51">
         <v>2013</v>
       </c>
       <c r="E51" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -6955,13 +6965,13 @@
         <v>122</v>
       </c>
       <c r="C52" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D52">
         <v>2014</v>
       </c>
       <c r="E52" s="2" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -6973,7 +6983,7 @@
         <v>115</v>
       </c>
       <c r="C53" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D53">
         <v>1997</v>
@@ -6988,13 +6998,13 @@
         <v>128</v>
       </c>
       <c r="C54" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D54">
         <v>2003</v>
       </c>
       <c r="E54" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -7033,13 +7043,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
+        <v>331</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>332</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="C1" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="C1" s="9" t="s">
-        <v>334</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -7047,10 +7057,10 @@
         <v>43080</v>
       </c>
       <c r="B2" s="10" t="s">
+        <v>334</v>
+      </c>
+      <c r="C2" s="10" t="s">
         <v>335</v>
-      </c>
-      <c r="C2" s="10" t="s">
-        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -7114,19 +7124,19 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="12" t="s">
+        <v>336</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>337</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>338</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>339</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="12" t="s">
         <v>340</v>
-      </c>
-      <c r="E1" s="12" t="s">
-        <v>341</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -7134,169 +7144,169 @@
         <v>130</v>
       </c>
       <c r="B2" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C2" s="14" t="s">
+        <v>356</v>
+      </c>
+      <c r="D2" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C2" s="14" t="s">
-        <v>357</v>
-      </c>
-      <c r="D2" s="13" t="s">
+      <c r="E2" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="E2" s="13" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B3" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>344</v>
+      </c>
+      <c r="D3" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C3" s="13" t="s">
-        <v>345</v>
-      </c>
-      <c r="D3" s="13" t="s">
+      <c r="E3" s="13" t="s">
         <v>343</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="10" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="B4" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>484</v>
+      </c>
+      <c r="D4" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C4" s="13" t="s">
-        <v>485</v>
-      </c>
-      <c r="D4" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E4" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="10" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B5" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C5" s="13" t="s">
+        <v>477</v>
+      </c>
+      <c r="D5" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C5" s="13" t="s">
-        <v>478</v>
-      </c>
-      <c r="D5" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E5" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B6" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>483</v>
+      </c>
+      <c r="D6" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C6" s="13" t="s">
-        <v>484</v>
-      </c>
-      <c r="D6" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E6" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="10" t="s">
+        <v>475</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C7" s="13" t="s">
         <v>476</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="D7" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C7" s="13" t="s">
-        <v>477</v>
-      </c>
-      <c r="D7" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E7" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="10" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="B8" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>485</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>486</v>
-      </c>
-      <c r="D8" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E8" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="10" t="s">
+        <v>478</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C9" s="13" t="s">
         <v>479</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="D9" s="13" t="s">
         <v>342</v>
       </c>
-      <c r="C9" s="13" t="s">
-        <v>480</v>
-      </c>
-      <c r="D9" s="13" t="s">
-        <v>343</v>
-      </c>
       <c r="E9" s="13" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="13" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B10" s="13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="14" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B11" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>354</v>
+      </c>
+      <c r="D11" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="C11" s="13" t="s">
-        <v>355</v>
-      </c>
-      <c r="D11" s="14" t="s">
+      <c r="E11" s="14" t="s">
         <v>343</v>
-      </c>
-      <c r="E11" s="14" t="s">
-        <v>344</v>
       </c>
     </row>
     <row r="12" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
@@ -7304,50 +7314,50 @@
         <v>0</v>
       </c>
       <c r="B12" s="14" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D12" s="14" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E12" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="14" t="s">
+        <v>349</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>341</v>
+      </c>
+      <c r="C13" s="13" t="s">
         <v>350</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="D13" s="14" t="s">
         <v>342</v>
       </c>
-      <c r="C13" s="13" t="s">
-        <v>351</v>
-      </c>
-      <c r="D13" s="14" t="s">
-        <v>343</v>
-      </c>
       <c r="E13" s="14" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="13" t="s">
+        <v>351</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>341</v>
+      </c>
+      <c r="C14" s="13" t="s">
         <v>352</v>
       </c>
-      <c r="B14" s="13" t="s">
-        <v>342</v>
-      </c>
-      <c r="C14" s="13" t="s">
-        <v>353</v>
-      </c>
       <c r="D14" s="13" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E14" s="13" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
     </row>
   </sheetData>

</xml_diff>